<commit_message>
fix: register & update: create & edit merchant
</commit_message>
<xml_diff>
--- a/public/backend/format_upload/Format Bulk Upload Merchant.xlsx
+++ b/public/backend/format_upload/Format Bulk Upload Merchant.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayus\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\indopay\public\backend\format_upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A72D448-69D6-48DE-9114-2BD4267EA2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E6804B-8C4A-40FD-9DD4-80DE19CE0165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CB69192C-D26A-4EB6-AE8D-5DA203315B30}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Bulk Upload Merchant Indopay</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Rek Pooling Code</t>
+  </si>
+  <si>
+    <t>Merchant Type</t>
   </si>
 </sst>
 </file>
@@ -495,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD5FB8D-71DA-48AE-8889-DE81DB10C2CA}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,12 +521,12 @@
     <col min="14" max="14" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -531,52 +534,55 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="C4" s="3"/>
       <c r="I4" s="4"/>
@@ -587,5 +593,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug dan add change password
</commit_message>
<xml_diff>
--- a/public/backend/format_upload/Format Bulk Upload Merchant.xlsx
+++ b/public/backend/format_upload/Format Bulk Upload Merchant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\indopay\public\backend\format_upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E6804B-8C4A-40FD-9DD4-80DE19CE0165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EE2881-8736-4D31-ACF6-ED5ED31CEB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CB69192C-D26A-4EB6-AE8D-5DA203315B30}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Bulk Upload Merchant Indopay</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>Merchant Type</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>Sub district</t>
+  </si>
+  <si>
+    <t>Village</t>
   </si>
 </sst>
 </file>
@@ -498,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD5FB8D-71DA-48AE-8889-DE81DB10C2CA}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,8 +521,9 @@
     <col min="4" max="4" width="28.28515625" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
@@ -521,12 +531,12 @@
     <col min="14" max="14" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -543,46 +553,55 @@
         <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="C4" s="3"/>
       <c r="I4" s="4"/>

</xml_diff>